<commit_message>
Test whether RowFiller and ExcelMerger can be combined
It works, as long as there is no interference.
But it's perfectly fine to merge header data with ExcelMerger.mergeData
and then fill a large set of rows with the RowFiller.
</commit_message>
<xml_diff>
--- a/excelmerger-impl/src/test/resources/ch/dvbern/oss/lib/excelmerger/sxssf.xlsx
+++ b/excelmerger-impl/src/test/resources/ch/dvbern/oss/lib/excelmerger/sxssf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tarif" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">Hallo du Vogel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{name}</t>
   </si>
   <si>
     <t xml:space="preserve">{value1}</t>
@@ -212,31 +215,34 @@
   </sheetPr>
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="4"/>
       <c r="F1" s="5"/>
     </row>
@@ -248,17 +254,17 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4" t="e">
         <f aca="false">A3+B3</f>
         <v>#VALUE!</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -268,55 +274,55 @@
         <v>#VALUE!</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>4</v>
-      </c>
       <c r="O3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="S3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>